<commit_message>
- Back at doing GD! - Simplifying Fighter skills and changing some of those skill effect and removing some specific effect.
- Will Simplify every class to cut some effect and make learning curve easier.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
+++ b/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-FighterMeditation" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="9-KiBlast" sheetId="11" r:id="rId9"/>
     <sheet name="10-LiquidKick" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t xml:space="preserve">Fighter Meditation </t>
   </si>
@@ -153,9 +153,6 @@
     <t xml:space="preserve">Increases the target's AP and power.                                       Remove the Fighter Meditation effect if the target has it.   </t>
   </si>
   <si>
-    <t>Move in the opposite direction from target by 1 cell.</t>
-  </si>
-  <si>
     <t>Teleports onto the targeted empty cell.</t>
   </si>
   <si>
@@ -178,72 +175,6 @@
   </si>
   <si>
     <t>Else:</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Precision Strike]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +2 levels (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    [[Precision Strike]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +1 level (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[[Damage:  (20 * </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Precision Strike]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> levels) wind ]]</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Reduces an enemy resistance.                                                         </t>
@@ -320,62 +251,6 @@
     <t xml:space="preserve">    [[Damage: 1-100 light ]]</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Self: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Kick]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +1 level (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Self: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Punch]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +1 level (1 turn)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">    Push 2 cells.</t>
   </si>
   <si>
@@ -383,69 +258,6 @@
   </si>
   <si>
     <t>If targeting an enemy:</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If self as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Fighter Aura]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If the target as </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Fighter Meditation]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
   </si>
   <si>
     <t>Inflicts Wind-type damage.                                                                   The damage dealt keep increasing if the skill is chained on the target.                                                                                                The damage increase faster if the caster as Fighter Aura effect.</t>
@@ -507,7 +319,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t>[[Vulnerability]]</t>
+      <t>[[Incurable]]</t>
     </r>
     <r>
       <rPr>
@@ -516,8 +328,11 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> +10 levels (1 turn)</t>
+      <t xml:space="preserve"> (2 turns)</t>
     </r>
+  </si>
+  <si>
+    <t>[[Damage:  20 wind ]]</t>
   </si>
   <si>
     <r>
@@ -527,7 +342,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">    [[Vulnerability]]</t>
+      <t>[[Power]]</t>
     </r>
     <r>
       <rPr>
@@ -536,14 +351,53 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> +20 levels (1 turn) (50%)</t>
+      <t xml:space="preserve"> +15 levels (10 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[[Preparation]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+25 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Move in the opposite direction from target by 2 cells.</t>
+  </si>
+  <si>
+    <t>At adjacent target;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Under-Power]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (1 turn) (50%)</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -737,6 +591,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,14 +905,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1153,14 +1008,14 @@
     <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1204,14 +1059,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1240,7 +1095,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1304,73 +1159,66 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="13" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="14" t="s">
-        <v>72</v>
+      <c r="C17" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="13" t="s">
-        <v>68</v>
+      <c r="C18" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="18" t="s">
-        <v>69</v>
+      <c r="C19" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="9"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1379,14 +1227,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1482,14 +1330,14 @@
     <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1533,14 +1381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1569,7 +1417,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1647,45 +1495,52 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="16" t="s">
+        <v>64</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="9"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1694,14 +1549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="89.7109375" customWidth="1"/>
@@ -1730,7 +1585,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1797,70 +1652,56 @@
     <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="16" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="18" t="s">
-        <v>50</v>
+      <c r="C18" s="20" t="s">
+        <v>67</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="1"/>
-      <c r="C20" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B26" s="1"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="9"/>
+      <c r="D25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1869,14 +1710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1905,7 +1746,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1968,81 +1809,67 @@
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="5" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B27" s="1"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="9"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2051,14 +1878,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2087,7 +1914,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2161,56 +1988,49 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="5" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="9"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2219,14 +2039,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2255,7 +2075,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2387,14 +2207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2423,7 +2243,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2509,14 +2329,14 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2560,14 +2380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2596,7 +2416,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2677,42 +2497,42 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1"/>
     </row>

</xml_diff>

<commit_message>
- Added Focus skill. - Added Vulnerability, Incurable, Vitality effect.
- Next task is to continue to add the skills of the fighter and the effects used by them.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
+++ b/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-FighterMeditation" sheetId="2" r:id="rId1"/>
@@ -1062,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1384,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Added Precision Strike, Slide, Strategic Retraite, Eagle Flight Skill. - Added Preparation and Power Effect.
- Next task is to continue to add Fighter skill and effect.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
+++ b/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-FighterMeditation" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t xml:space="preserve">Fighter Meditation </t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Inflicts Ground-type damage to enemies.                                                            Move the caster in front of the target.                                      Increases the next Liquid Kick damage.</t>
-  </si>
-  <si>
-    <t>[[Damage:  27-30 ground ]]</t>
   </si>
   <si>
     <t>Inflicts Ground-type damage.                                                              Can only be used on enemies.                                                        Move the caster in the opposite direction.                               Increase the next Iron Punch damage.</t>
@@ -392,6 +389,9 @@
       </rPr>
       <t xml:space="preserve"> +25 levels (1 turn) (50%)</t>
     </r>
+  </si>
+  <si>
+    <t>[[Damage: 30 ground ]]</t>
   </si>
 </sst>
 </file>
@@ -1008,14 +1008,14 @@
     <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1169,21 +1169,21 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1330,14 +1330,14 @@
     <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
       <c r="C16" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1383,503 +1383,6 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="1"/>
-      <c r="C18" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="1"/>
-      <c r="C19" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B23" s="1"/>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:D25"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="89.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="1"/>
-      <c r="C16" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="1"/>
-      <c r="C17" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="1"/>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1"/>
-      <c r="C7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B23" s="1"/>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
@@ -1902,7 +1405,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1911,10 +1414,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="11" t="s">
-        <v>45</v>
+      <c r="C5" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1926,7 +1429,175 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="5" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="1"/>
+      <c r="C18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="1"/>
+      <c r="C19" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="1"/>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B2:D25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="89.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -1957,6 +1628,342 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="1"/>
+      <c r="C16" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="1"/>
+      <c r="C17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B2:D27"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B26" s="1"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B2:D25"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="1"/>
@@ -1988,14 +1995,14 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="5" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2042,7 +2049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2243,7 +2250,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2329,14 +2336,14 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2416,7 +2423,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2497,42 +2504,42 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1"/>
     </row>

</xml_diff>

<commit_message>
- Added Iron Punch, Ki Blast, Liquid Kick Skills. - Added Powerless and Under-power Effects. - Minor change in Fighter skills documentation.
- Next task is to create 3 test equipment for every kind of equipment.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
+++ b/GameDesign/Class/_Done/1_Fighter/Documentation/FighterSkills.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="864" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-FighterMeditation" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
   <si>
     <t xml:space="preserve">Fighter Meditation </t>
   </si>
@@ -1060,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,111 +1114,118 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="13" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B19" s="1"/>
+      <c r="C19" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="1"/>
-      <c r="C19" s="14" t="s">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="1"/>
+      <c r="C20" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="1"/>
+      <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="8"/>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="9"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2049,7 +2056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2218,7 +2225,7 @@
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,7 +2397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>

</xml_diff>